<commit_message>
update exercises-3 to be clearer
</commit_message>
<xml_diff>
--- a/topic03-microsoft-excel/unit-3-labs-week-7/archive-2/exercise-3/Exercises-3.xlsx
+++ b/topic03-microsoft-excel/unit-3-labs-week-7/archive-2/exercise-3/Exercises-3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maireadmeagher/Documents/GitRepos/ICT-25/topic03-microsoft-excel/unit-3-labs-week-7/archive-2/exercise-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F6322F-BBB7-ED42-81F8-21F947402A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FBC735-EB0C-3E42-BD40-31C5C8E4BC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" tabRatio="749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17760" tabRatio="749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PloughingChampionship" sheetId="20" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>Year</t>
   </si>
@@ -234,9 +234,6 @@
     <t>Part 1</t>
   </si>
   <si>
-    <t>Calculate each students correct weighted result and then the overall average.</t>
-  </si>
-  <si>
     <t>Overall</t>
   </si>
   <si>
@@ -259,15 +256,6 @@
   </si>
   <si>
     <t>Part 2</t>
-  </si>
-  <si>
-    <t>Present all the information/values from part 1, SORT THE DATA, by surname</t>
-  </si>
-  <si>
-    <t>and calculate all values again with exam weights of      .1,    .3,   .6 respectively</t>
-  </si>
-  <si>
-    <t>Omit the 4th student from the Overall average answer.</t>
   </si>
   <si>
     <t xml:space="preserve">Student Results -weighting of marks, sorting, conditional formatting. </t>
@@ -388,6 +376,16 @@
 The data should be sorted on name in ascending order.
 Part 3) 
 Copy the details again (with weightings) from Part 1. This time, sort based on the overall mark in Descending order. 
+</t>
+  </si>
+  <si>
+    <t>Calculate each students correct weighted result and then the overall average.
+Then apply conditional formatting as per instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present all the information/values from part 1, SORT THE DATA, by surname
+Apply new weightings as per instructions,
+Apply contitional formatting as per instructions. 
 </t>
   </si>
 </sst>
@@ -870,7 +868,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1128,6 +1126,48 @@
     <border>
       <left/>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1139,6 +1179,15 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1168,6 +1217,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1175,9 +1244,47 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1330,7 +1437,7 @@
     <xf numFmtId="0" fontId="31" fillId="20" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1427,9 +1534,8 @@
     </xf>
     <xf numFmtId="2" fontId="36" fillId="19" borderId="16" xfId="72" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1450,10 +1556,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1476,10 +1582,10 @@
     <xf numFmtId="0" fontId="5" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="43" fillId="18" borderId="22" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="43" fillId="18" borderId="27" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="43" fillId="18" borderId="2" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1491,7 +1597,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1512,14 +1618,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="33" xfId="73" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="75">
@@ -2059,14 +2235,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="19">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
       <c r="H1" s="5"/>
       <c r="I1" s="3"/>
     </row>
@@ -2865,8 +3041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AED8B6-C8E4-1946-80AA-C7F047103217}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2881,19 +3057,19 @@
     <col min="11" max="11" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="16" thickBot="1">
       <c r="A1" s="28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="21">
       <c r="A2" s="28"/>
       <c r="C2" s="38" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G2" s="39"/>
       <c r="M2" s="89" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N2" s="90"/>
       <c r="O2" s="90"/>
@@ -2903,444 +3079,467 @@
       <c r="S2" s="90"/>
       <c r="T2" s="90"/>
       <c r="U2" s="90"/>
-      <c r="V2" s="90"/>
+      <c r="V2" s="91"/>
     </row>
     <row r="3" spans="1:22" ht="31.25" customHeight="1">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="39"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="90"/>
-      <c r="R3" s="90"/>
-      <c r="S3" s="90"/>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="93"/>
+      <c r="T3" s="93"/>
+      <c r="U3" s="93"/>
+      <c r="V3" s="94"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="39"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-    </row>
-    <row r="5" spans="1:22" ht="21" customHeight="1">
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="90"/>
-      <c r="Q5" s="90"/>
-      <c r="R5" s="90"/>
-      <c r="S5" s="90"/>
-      <c r="T5" s="90"/>
-      <c r="U5" s="90"/>
-      <c r="V5" s="90"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="93"/>
+      <c r="Q4" s="93"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
+      <c r="V4" s="94"/>
+    </row>
+    <row r="5" spans="1:22" ht="4" customHeight="1">
+      <c r="M5" s="92"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="93"/>
+      <c r="Q5" s="93"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="93"/>
+      <c r="T5" s="93"/>
+      <c r="U5" s="93"/>
+      <c r="V5" s="94"/>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="100" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="102"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
+      <c r="P6" s="93"/>
+      <c r="Q6" s="93"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="93"/>
+      <c r="T6" s="93"/>
+      <c r="U6" s="93"/>
+      <c r="V6" s="94"/>
+    </row>
+    <row r="7" spans="1:22" ht="32" customHeight="1">
+      <c r="A7" s="41"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="104"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
+      <c r="O7" s="93"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="93"/>
+      <c r="U7" s="93"/>
+      <c r="V7" s="94"/>
+    </row>
+    <row r="8" spans="1:22" s="36" customFormat="1" ht="32">
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="90"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="90"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="90"/>
-      <c r="V6" s="90"/>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="41"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="90"/>
-      <c r="S7" s="90"/>
-      <c r="T7" s="90"/>
-      <c r="U7" s="90"/>
-      <c r="V7" s="90"/>
-    </row>
-    <row r="8" spans="1:22" s="36" customFormat="1" ht="32">
-      <c r="A8" s="84"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="88" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="88" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="88" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="88" t="s">
+      <c r="M8" s="92"/>
+      <c r="N8" s="93"/>
+      <c r="O8" s="93"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="93"/>
+      <c r="T8" s="93"/>
+      <c r="U8" s="93"/>
+      <c r="V8" s="94"/>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
-      <c r="O8" s="90"/>
-      <c r="P8" s="90"/>
-      <c r="Q8" s="90"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="90"/>
-      <c r="U8" s="90"/>
-      <c r="V8" s="90"/>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="85" t="s">
+      <c r="B9" s="85"/>
+      <c r="C9" s="86">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="86">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="86">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="86">
+        <v>1</v>
+      </c>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
+      <c r="O9" s="93"/>
+      <c r="P9" s="93"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
+      <c r="S9" s="93"/>
+      <c r="T9" s="93"/>
+      <c r="U9" s="93"/>
+      <c r="V9" s="94"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="M10" s="92"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="93"/>
+      <c r="R10" s="93"/>
+      <c r="S10" s="93"/>
+      <c r="T10" s="93"/>
+      <c r="U10" s="93"/>
+      <c r="V10" s="94"/>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="87">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="87">
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="87">
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="87">
-        <v>0.1</v>
-      </c>
-      <c r="G9" s="87">
-        <v>1</v>
-      </c>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="90"/>
-      <c r="S9" s="90"/>
-      <c r="T9" s="90"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="90"/>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A10" s="86"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
-      <c r="O10" s="90"/>
-      <c r="P10" s="90"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="90"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="90"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="90"/>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="86" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86">
+      <c r="B11" s="85"/>
+      <c r="C11" s="85">
         <v>67</v>
       </c>
-      <c r="D11" s="86">
+      <c r="D11" s="85">
         <v>23</v>
       </c>
-      <c r="E11" s="86">
+      <c r="E11" s="85">
         <v>56</v>
       </c>
-      <c r="F11" s="86">
+      <c r="F11" s="85">
         <v>78</v>
       </c>
-      <c r="G11" s="86"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="90"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="90"/>
-      <c r="V11" s="90"/>
+      <c r="G11" s="85"/>
+      <c r="M11" s="92"/>
+      <c r="N11" s="93"/>
+      <c r="O11" s="93"/>
+      <c r="P11" s="93"/>
+      <c r="Q11" s="93"/>
+      <c r="R11" s="93"/>
+      <c r="S11" s="93"/>
+      <c r="T11" s="93"/>
+      <c r="U11" s="93"/>
+      <c r="V11" s="94"/>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86">
+        <v>68</v>
+      </c>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85">
         <v>24</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="85">
         <v>39</v>
       </c>
-      <c r="E12" s="86">
+      <c r="E12" s="85">
         <v>23</v>
       </c>
-      <c r="F12" s="86">
+      <c r="F12" s="85">
         <v>56</v>
       </c>
-      <c r="G12" s="86"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="90"/>
-      <c r="U12" s="90"/>
-      <c r="V12" s="90"/>
+      <c r="G12" s="85"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="93"/>
+      <c r="O12" s="93"/>
+      <c r="P12" s="93"/>
+      <c r="Q12" s="93"/>
+      <c r="R12" s="93"/>
+      <c r="S12" s="93"/>
+      <c r="T12" s="93"/>
+      <c r="U12" s="93"/>
+      <c r="V12" s="94"/>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85">
+        <v>40</v>
+      </c>
+      <c r="D13" s="85">
+        <v>60</v>
+      </c>
+      <c r="E13" s="85">
+        <v>44</v>
+      </c>
+      <c r="F13" s="85">
+        <v>67</v>
+      </c>
+      <c r="G13" s="85"/>
+      <c r="K13" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86">
-        <v>40</v>
-      </c>
-      <c r="D13" s="86">
-        <v>60</v>
-      </c>
-      <c r="E13" s="86">
-        <v>44</v>
-      </c>
-      <c r="F13" s="86">
+      <c r="M13" s="92"/>
+      <c r="N13" s="93"/>
+      <c r="O13" s="93"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="93"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="93"/>
+      <c r="T13" s="93"/>
+      <c r="U13" s="93"/>
+      <c r="V13" s="94"/>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85">
+        <v>33</v>
+      </c>
+      <c r="D14" s="85">
+        <v>46</v>
+      </c>
+      <c r="E14" s="85">
+        <v>55</v>
+      </c>
+      <c r="F14" s="85">
         <v>67</v>
       </c>
-      <c r="G13" s="86"/>
-      <c r="K13" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="90"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
-      <c r="V13" s="90"/>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="86" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86">
-        <v>33</v>
-      </c>
-      <c r="D14" s="86">
-        <v>46</v>
-      </c>
-      <c r="E14" s="86">
-        <v>55</v>
-      </c>
-      <c r="F14" s="86">
-        <v>67</v>
-      </c>
-      <c r="G14" s="86"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="90"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="90"/>
+      <c r="G14" s="85"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="93"/>
+      <c r="O14" s="93"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="93"/>
+      <c r="R14" s="93"/>
+      <c r="S14" s="93"/>
+      <c r="T14" s="93"/>
+      <c r="U14" s="93"/>
+      <c r="V14" s="94"/>
     </row>
     <row r="15" spans="1:22" ht="16" thickBot="1">
-      <c r="A15" s="86" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86">
+      <c r="A15" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85">
         <v>23</v>
       </c>
-      <c r="D15" s="86">
+      <c r="D15" s="85">
         <v>45</v>
       </c>
-      <c r="E15" s="86">
+      <c r="E15" s="85">
         <v>12</v>
       </c>
-      <c r="F15" s="86">
+      <c r="F15" s="85">
         <v>77</v>
       </c>
-      <c r="G15" s="86"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="90"/>
-      <c r="O15" s="90"/>
-      <c r="P15" s="90"/>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="90"/>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
-      <c r="U15" s="90"/>
-      <c r="V15" s="90"/>
+      <c r="G15" s="85"/>
+      <c r="M15" s="92"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="93"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="93"/>
+      <c r="T15" s="93"/>
+      <c r="U15" s="93"/>
+      <c r="V15" s="94"/>
     </row>
     <row r="16" spans="1:22" ht="25" thickBot="1">
       <c r="H16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K16" s="44"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="90"/>
-      <c r="O16" s="90"/>
-      <c r="P16" s="90"/>
-      <c r="Q16" s="90"/>
-      <c r="R16" s="90"/>
-      <c r="S16" s="90"/>
-      <c r="T16" s="90"/>
-      <c r="U16" s="90"/>
-      <c r="V16" s="90"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="93"/>
+      <c r="T16" s="93"/>
+      <c r="U16" s="93"/>
+      <c r="V16" s="94"/>
     </row>
     <row r="17" spans="1:22" ht="18.75" customHeight="1">
       <c r="K17" s="45"/>
-      <c r="M17" s="90"/>
-      <c r="N17" s="90"/>
-      <c r="O17" s="90"/>
-      <c r="P17" s="90"/>
-      <c r="Q17" s="90"/>
-      <c r="R17" s="90"/>
-      <c r="S17" s="90"/>
-      <c r="T17" s="90"/>
-      <c r="U17" s="90"/>
-      <c r="V17" s="90"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="93"/>
+      <c r="R17" s="93"/>
+      <c r="S17" s="93"/>
+      <c r="T17" s="93"/>
+      <c r="U17" s="93"/>
+      <c r="V17" s="94"/>
     </row>
     <row r="18" spans="1:22" ht="16" thickBot="1">
       <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="88"/>
       <c r="I18" s="46"/>
       <c r="J18" s="46"/>
       <c r="K18" s="47"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="90"/>
-      <c r="P18" s="90"/>
-      <c r="Q18" s="90"/>
-      <c r="R18" s="90"/>
-      <c r="S18" s="90"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
+      <c r="M18" s="92"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="93"/>
+      <c r="P18" s="93"/>
+      <c r="Q18" s="93"/>
+      <c r="R18" s="93"/>
+      <c r="S18" s="93"/>
+      <c r="T18" s="93"/>
+      <c r="U18" s="93"/>
+      <c r="V18" s="94"/>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
+      <c r="A19" s="105" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="100" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="109"/>
       <c r="K19" s="45"/>
-      <c r="M19" s="90"/>
-      <c r="N19" s="90"/>
-      <c r="O19" s="90"/>
-      <c r="P19" s="90"/>
-      <c r="Q19" s="90"/>
-      <c r="R19" s="90"/>
-      <c r="S19" s="90"/>
-      <c r="T19" s="90"/>
-      <c r="U19" s="90"/>
-      <c r="V19" s="90"/>
+      <c r="M19" s="92"/>
+      <c r="N19" s="93"/>
+      <c r="O19" s="93"/>
+      <c r="P19" s="93"/>
+      <c r="Q19" s="93"/>
+      <c r="R19" s="93"/>
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="93"/>
+      <c r="V19" s="94"/>
     </row>
     <row r="20" spans="1:22">
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
+      <c r="B20" s="110"/>
+      <c r="C20" s="111"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="112"/>
       <c r="K20" s="45"/>
-      <c r="M20" s="90"/>
-      <c r="N20" s="90"/>
-      <c r="O20" s="90"/>
-      <c r="P20" s="90"/>
-      <c r="Q20" s="90"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="90"/>
-      <c r="T20" s="90"/>
-      <c r="U20" s="90"/>
-      <c r="V20" s="90"/>
+      <c r="M20" s="92"/>
+      <c r="N20" s="93"/>
+      <c r="O20" s="93"/>
+      <c r="P20" s="93"/>
+      <c r="Q20" s="93"/>
+      <c r="R20" s="93"/>
+      <c r="S20" s="93"/>
+      <c r="T20" s="93"/>
+      <c r="U20" s="93"/>
+      <c r="V20" s="94"/>
     </row>
     <row r="21" spans="1:22">
-      <c r="B21" s="48" t="s">
-        <v>39</v>
-      </c>
+      <c r="B21" s="113"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="114"/>
       <c r="K21" s="45"/>
-      <c r="M21" s="90"/>
-      <c r="N21" s="90"/>
-      <c r="O21" s="90"/>
-      <c r="P21" s="90"/>
-      <c r="Q21" s="90"/>
-      <c r="R21" s="90"/>
-      <c r="S21" s="90"/>
-      <c r="T21" s="90"/>
-      <c r="U21" s="90"/>
-      <c r="V21" s="90"/>
-    </row>
-    <row r="22" spans="1:22" ht="34" customHeight="1">
-      <c r="C22" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="91" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="91" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="91" t="s">
-        <v>29</v>
+      <c r="M21" s="92"/>
+      <c r="N21" s="93"/>
+      <c r="O21" s="93"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="93"/>
+      <c r="R21" s="93"/>
+      <c r="S21" s="93"/>
+      <c r="T21" s="93"/>
+      <c r="U21" s="93"/>
+      <c r="V21" s="94"/>
+    </row>
+    <row r="22" spans="1:22" ht="34" customHeight="1" thickBot="1">
+      <c r="C22" s="106" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="107" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="107" t="s">
+        <v>28</v>
       </c>
       <c r="K22" s="45"/>
-      <c r="M22" s="90"/>
-      <c r="N22" s="90"/>
-      <c r="O22" s="90"/>
-      <c r="P22" s="90"/>
-      <c r="Q22" s="90"/>
-      <c r="R22" s="90"/>
-      <c r="S22" s="90"/>
-      <c r="T22" s="90"/>
-      <c r="U22" s="90"/>
-      <c r="V22" s="90"/>
+      <c r="M22" s="95"/>
+      <c r="N22" s="96"/>
+      <c r="O22" s="96"/>
+      <c r="P22" s="96"/>
+      <c r="Q22" s="96"/>
+      <c r="R22" s="96"/>
+      <c r="S22" s="96"/>
+      <c r="T22" s="96"/>
+      <c r="U22" s="96"/>
+      <c r="V22" s="97"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K23" s="45"/>
     </row>
@@ -3351,16 +3550,16 @@
       <c r="K24" s="45"/>
     </row>
     <row r="28" spans="1:22" ht="16" thickBot="1">
-      <c r="A28" s="49"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
     </row>
     <row r="29" spans="1:22" ht="25" thickBot="1">
       <c r="H29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K29" s="44"/>
     </row>
@@ -3371,8 +3570,10 @@
       <c r="K31" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="M2:V22"/>
+    <mergeCell ref="B19:H21"/>
+    <mergeCell ref="C6:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3394,369 +3595,369 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+    </row>
+    <row r="2" spans="1:17" ht="16">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+    </row>
+    <row r="3" spans="1:17" ht="17" thickBot="1">
+      <c r="A3" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="49"/>
+    </row>
+    <row r="4" spans="1:17" ht="20" thickBot="1">
+      <c r="A4" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-    </row>
-    <row r="2" spans="1:17" ht="16">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-    </row>
-    <row r="3" spans="1:17" ht="17" thickBot="1">
-      <c r="A3" s="51" t="s">
+      <c r="J4" s="56"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+    </row>
+    <row r="5" spans="1:17" ht="19">
+      <c r="A5" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="50"/>
-    </row>
-    <row r="4" spans="1:17" ht="20" thickBot="1">
-      <c r="A4" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="57"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-    </row>
-    <row r="5" spans="1:17" ht="19">
-      <c r="A5" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="60">
+      <c r="B5" s="59">
         <v>5</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="19">
         <v>1</v>
       </c>
-      <c r="F5" s="61" t="s">
-        <v>47</v>
+      <c r="F5" s="60" t="s">
+        <v>43</v>
       </c>
       <c r="G5" s="39"/>
       <c r="H5" s="39"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
     </row>
     <row r="6" spans="1:17" ht="19">
-      <c r="A6" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="64">
+      <c r="A6" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="63">
         <v>10</v>
       </c>
-      <c r="D6" s="54"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="19">
         <v>2</v>
       </c>
-      <c r="F6" s="65" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="62"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
+      <c r="F6" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="61"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
     </row>
     <row r="7" spans="1:17" ht="19">
-      <c r="A7" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="64">
+      <c r="A7" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="63">
         <v>8</v>
       </c>
-      <c r="D7" s="54"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="19">
         <v>3</v>
       </c>
-      <c r="F7" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="66"/>
+      <c r="F7" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="61"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="65"/>
     </row>
     <row r="8" spans="1:17" ht="19">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="D8" s="54"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="19">
         <v>4</v>
       </c>
-      <c r="F8" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
+      <c r="F8" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
     </row>
     <row r="9" spans="1:17" ht="20" thickBot="1">
-      <c r="A9" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="50"/>
-      <c r="D9" s="54"/>
+      <c r="A9" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="D9" s="53"/>
       <c r="E9" s="19">
         <v>5</v>
       </c>
-      <c r="F9" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
+      <c r="F9" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
     </row>
     <row r="10" spans="1:17" ht="20" thickBot="1">
-      <c r="A10" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="54"/>
+      <c r="A10" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="53"/>
       <c r="E10" s="19">
         <v>6</v>
       </c>
-      <c r="F10" s="61" t="s">
+      <c r="F10" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+    </row>
+    <row r="11" spans="1:17" ht="19">
+      <c r="A11" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="59">
+        <v>500</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="67">
+        <v>7</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="20" thickBot="1">
+      <c r="A12" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="63">
+        <v>900</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="68">
+        <v>8</v>
+      </c>
+      <c r="F12" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-    </row>
-    <row r="11" spans="1:17" ht="19">
-      <c r="A11" s="60" t="s">
+    </row>
+    <row r="13" spans="1:17" ht="18">
+      <c r="A13" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="60">
-        <v>500</v>
-      </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="68">
-        <v>7</v>
-      </c>
-      <c r="F11" s="65" t="s">
+      <c r="B13" s="63">
+        <v>1200</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="E13" s="66"/>
+    </row>
+    <row r="14" spans="1:17" ht="18">
+      <c r="A14" s="63" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="20" thickBot="1">
-      <c r="A12" s="64" t="s">
+      <c r="B14" s="63">
+        <v>600</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="E14" s="66"/>
+    </row>
+    <row r="15" spans="1:17" ht="18">
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="66"/>
+    </row>
+    <row r="16" spans="1:17" ht="19" thickBot="1">
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="66"/>
+    </row>
+    <row r="17" spans="1:17" ht="18">
+      <c r="A17" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="64">
-        <v>900</v>
-      </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="69">
-        <v>8</v>
-      </c>
-      <c r="F12" s="70" t="s">
+      <c r="B17" s="71"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="66"/>
+    </row>
+    <row r="18" spans="1:17" ht="18">
+      <c r="A18" s="73" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="18">
-      <c r="A13" s="64" t="s">
+      <c r="B18" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="64">
-        <v>1200</v>
-      </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="67"/>
-    </row>
-    <row r="14" spans="1:17" ht="18">
-      <c r="A14" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="64">
-        <v>600</v>
-      </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="67"/>
-    </row>
-    <row r="15" spans="1:17" ht="18">
-      <c r="A15" s="50"/>
-      <c r="B15" s="50"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="67"/>
-    </row>
-    <row r="16" spans="1:17" ht="19" thickBot="1">
-      <c r="A16" s="50"/>
-      <c r="B16" s="50"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="67"/>
-    </row>
-    <row r="17" spans="1:17" ht="18">
-      <c r="A17" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="67"/>
-    </row>
-    <row r="18" spans="1:17" ht="18">
-      <c r="A18" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="75" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="67"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="66"/>
     </row>
     <row r="19" spans="1:17" ht="18">
-      <c r="A19" s="60">
+      <c r="A19" s="59">
         <v>2018</v>
       </c>
-      <c r="B19" s="76">
+      <c r="B19" s="75">
         <v>980</v>
       </c>
-      <c r="D19" s="54"/>
-      <c r="E19" s="67"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="66"/>
     </row>
     <row r="20" spans="1:17" ht="18">
-      <c r="A20" s="64">
+      <c r="A20" s="63">
         <f>A19+1</f>
         <v>2019</v>
       </c>
-      <c r="B20" s="77">
+      <c r="B20" s="76">
         <v>1100</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="67"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="66"/>
     </row>
     <row r="21" spans="1:17" ht="18">
-      <c r="A21" s="64">
+      <c r="A21" s="63">
         <f t="shared" ref="A21:A26" si="0">A20+1</f>
         <v>2020</v>
       </c>
-      <c r="B21" s="77">
+      <c r="B21" s="76">
         <v>1400</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="67"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="66"/>
     </row>
     <row r="22" spans="1:17" ht="18">
-      <c r="A22" s="64">
+      <c r="A22" s="63">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="B22" s="77">
+      <c r="B22" s="76">
         <v>1123</v>
       </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="67"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="82"/>
-      <c r="M22" s="82"/>
-      <c r="N22" s="82"/>
-      <c r="O22" s="82"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="82"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="66"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="81"/>
+      <c r="N22" s="81"/>
+      <c r="O22" s="81"/>
+      <c r="P22" s="81"/>
+      <c r="Q22" s="81"/>
     </row>
     <row r="23" spans="1:17" ht="16">
-      <c r="A23" s="64">
+      <c r="A23" s="63">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="B23" s="77">
+      <c r="B23" s="76">
         <v>1670</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="83"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
     </row>
     <row r="24" spans="1:17" ht="16">
-      <c r="A24" s="64">
+      <c r="A24" s="63">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="B24" s="77">
+      <c r="B24" s="76">
         <v>2005</v>
       </c>
-      <c r="D24" s="54"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="83"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
     </row>
     <row r="25" spans="1:17" ht="16">
-      <c r="A25" s="64">
+      <c r="A25" s="63">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="B25" s="77">
+      <c r="B25" s="76">
         <v>2500</v>
       </c>
-      <c r="D25" s="54"/>
+      <c r="D25" s="53"/>
     </row>
     <row r="26" spans="1:17" ht="18">
-      <c r="A26" s="64">
+      <c r="A26" s="63">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
-      <c r="B26" s="77">
+      <c r="B26" s="76">
         <v>2790</v>
       </c>
-      <c r="D26" s="54"/>
-      <c r="E26" s="67"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="66"/>
     </row>
     <row r="27" spans="1:17" ht="18">
-      <c r="A27" s="64"/>
-      <c r="B27" s="77"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="78"/>
+      <c r="A27" s="63"/>
+      <c r="B27" s="76"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>